<commit_message>
dataprovider placed in seperate class
</commit_message>
<xml_diff>
--- a/testdata/loginData.xlsx
+++ b/testdata/loginData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -40,12 +40,19 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -392,9 +399,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -415,6 +422,9 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
@@ -423,6 +433,9 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
@@ -431,6 +444,9 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
@@ -438,6 +454,9 @@
       </c>
       <c r="B5" t="s">
         <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>